<commit_message>
Add Folha2 to NFC vs RFID.xlsx
</commit_message>
<xml_diff>
--- a/Pesquisa/NFC vs RFID.xlsx
+++ b/Pesquisa/NFC vs RFID.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Folha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
   <si>
     <t>RFID e NFC são duas tecnologias de comunicação sem fio estreitamente relacionadas que são usadas globalmente para uma grande quantidade de aplicativos, como controle de acesso, rastreamento de ativos e pagamentos sem contato. A RFID foi patenteada pela primeira vez em 1983 e é o precursor da NFC, então vamos começar por lá.</t>
   </si>
@@ -175,12 +176,150 @@
   </si>
   <si>
     <t>howpublished = {\url{https://nfc.today/advice/difference-nfc-rfid-explained}},</t>
+  </si>
+  <si>
+    <t>RFID</t>
+  </si>
+  <si>
+    <t>Frequências</t>
+  </si>
+  <si>
+    <t>Opera a 13,56MHz (mesma frequência que HF do RFID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Low Frequency (LF) 125 -134 kHz</t>
+  </si>
+  <si>
+    <t>High Frequency (HF)13.56 MHz</t>
+  </si>
+  <si>
+    <t>Ultra High Frequency (UHF) 856 MHz to 960 MHz)</t>
+  </si>
+  <si>
+    <t>Comunicação</t>
+  </si>
+  <si>
+    <t>Unidirecional ou bidirecional (P2P)</t>
+  </si>
+  <si>
+    <t>Unidirecional</t>
+  </si>
+  <si>
+    <t>Distância</t>
+  </si>
+  <si>
+    <t>até 30cm</t>
+  </si>
+  <si>
+    <t>LF - até 10cm</t>
+  </si>
+  <si>
+    <t>HF - até 30cm</t>
+  </si>
+  <si>
+    <t>UHF - até 100m</t>
+  </si>
+  <si>
+    <t>Componentes</t>
+  </si>
+  <si>
+    <t>Leitor NFC e tag NFC</t>
+  </si>
+  <si>
+    <t>Leitor RFID, tag RFID e ua antena</t>
+  </si>
+  <si>
+    <t>Equipado nos smartphones</t>
+  </si>
+  <si>
+    <t>Na maioria dos smartphones</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Ativo/Passivo</t>
+  </si>
+  <si>
+    <t>Passivo, ativado na presença de um leitor NFC</t>
+  </si>
+  <si>
+    <t>Passivo, ativado na presença de um leitor RFID.</t>
+  </si>
+  <si>
+    <t>Ativo, a tag tem uma fonte de energia própria.</t>
+  </si>
+  <si>
+    <t>Uso aplicacional</t>
+  </si>
+  <si>
+    <t>Propriedade desenvolvidas para pagamentos</t>
+  </si>
+  <si>
+    <t>Usado globalmente para gestão de stocks,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> móveis seguros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> manipulação de bagagem no aeroporto,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> identificação de gado entre outros</t>
+  </si>
+  <si>
+    <t>Multiplas digitalizações</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Capacidade das tags</t>
+  </si>
+  <si>
+    <t>Depende do tipo das tags</t>
+  </si>
+  <si>
+    <t>Normalmente os tipos mais comuns são:</t>
+  </si>
+  <si>
+    <t>Normalmente têm 96 bits no mínimo.</t>
+  </si>
+  <si>
+    <t>Pode haver extensão de memória e tipicamente</t>
+  </si>
+  <si>
+    <t>esta é até 512 bits. Mas pode haver tags que</t>
+  </si>
+  <si>
+    <t>disponibilizem mais e pode ser até 4K ou 8K bytes.</t>
+  </si>
+  <si>
+    <t>192 Bytes (Ultralight C)</t>
+  </si>
+  <si>
+    <t>1024 Bytes (Standard 1K)</t>
+  </si>
+  <si>
+    <t>http://blog.clove.co.uk/2012/06/20/near-field-communication-nfc-explained-the-complete-guide/</t>
+  </si>
+  <si>
+    <t>https://www.quora.com/How-much-data-can-be-stored-on-an-NFC-chip</t>
+  </si>
+  <si>
+    <t>https://blog.atlasrfidstore.com/types-of-memory-in-gen-2-uhf-rfid-tags</t>
+  </si>
+  <si>
+    <t>Nota sobre o NFC:</t>
+  </si>
+  <si>
+    <t>Comunicação fácil e intuitiva entre telemóveis e tags NFC.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,7 +337,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -206,14 +345,208 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,11 +827,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:B75"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,4 +1133,394 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8909DF13-165E-466B-BC97-9B2F7B9003AA}">
+  <dimension ref="B7:F69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="83.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
+      <c r="E7" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D12" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D13" s="27"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="28"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D15" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D17" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D18" s="22"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D19" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D20" s="21"/>
+      <c r="E20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D21" s="22"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D23" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D24" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E30" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E31" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>